<commit_message>
User Controller + Views hinzugefügt
</commit_message>
<xml_diff>
--- a/Excelsheet_Webproject.xlsx
+++ b/Excelsheet_Webproject.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Documents\Google Drive\HTL\4BHWII\SWP\Projekte\GitHub\NotizenProjekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forme\OneDrive\Desktop\Schual\SWP\GitHub\NotizenProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00009E13-3992-4562-B94E-ACC59ECE84C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00009E13-3992-4562-B94E-ACC59ECE84C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{34C74C50-1293-4BE5-9D85-039682E6FF43}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{FD55CC8F-81FA-4163-8113-51E07961513C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FD55CC8F-81FA-4163-8113-51E07961513C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <t>Grundlayout deisgned</t>
   </si>
   <si>
-    <t>User-Klasse</t>
+    <t>User- und Message Klasse</t>
   </si>
 </sst>
 </file>
@@ -512,16 +512,16 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="26.1328125" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="11"/>
+    <col min="8" max="8" width="26.08984375" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,7 +543,7 @@
       </c>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -563,7 +563,7 @@
       </c>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -582,7 +582,7 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -601,7 +601,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -620,7 +620,7 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -628,632 +628,632 @@
       <c r="G6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D7" s="2"/>
       <c r="G7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D8" s="2"/>
       <c r="G8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D9" s="2"/>
       <c r="G9" s="2"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D10" s="2"/>
       <c r="G10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D11" s="2"/>
       <c r="G11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D12" s="2"/>
       <c r="G12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D13" s="2"/>
       <c r="G13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D14" s="2"/>
       <c r="G14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D15" s="2"/>
       <c r="G15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D16" s="2"/>
       <c r="G16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D17" s="2"/>
       <c r="G17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D18" s="2"/>
       <c r="G18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D19" s="2"/>
       <c r="G19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D20" s="2"/>
       <c r="G20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D21" s="2"/>
       <c r="G21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D22" s="2"/>
       <c r="G22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D23" s="2"/>
       <c r="G23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D24" s="2"/>
       <c r="G24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D25" s="2"/>
       <c r="G25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D26" s="2"/>
       <c r="G26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D27" s="2"/>
       <c r="G27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D28" s="2"/>
       <c r="G28" s="2"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D29" s="2"/>
       <c r="G29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D30" s="2"/>
       <c r="G30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D31" s="2"/>
       <c r="G31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D32" s="2"/>
       <c r="G32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D33" s="2"/>
       <c r="G33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D34" s="2"/>
       <c r="G34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D35" s="2"/>
       <c r="G35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D36" s="2"/>
       <c r="G36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D37" s="2"/>
       <c r="G37" s="2"/>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D38" s="2"/>
       <c r="G38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D39" s="2"/>
       <c r="G39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D40" s="2"/>
       <c r="G40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D41" s="2"/>
       <c r="G41" s="2"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D42" s="2"/>
       <c r="G42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D43" s="2"/>
       <c r="G43" s="2"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D44" s="2"/>
       <c r="G44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D45" s="2"/>
       <c r="G45" s="2"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D46" s="2"/>
       <c r="G46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D47" s="2"/>
       <c r="G47" s="2"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D48" s="2"/>
       <c r="G48" s="2"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D49" s="2"/>
       <c r="G49" s="2"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D50" s="2"/>
       <c r="G50" s="2"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D51" s="2"/>
       <c r="G51" s="2"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D52" s="2"/>
       <c r="G52" s="2"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D53" s="2"/>
       <c r="G53" s="2"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D54" s="2"/>
       <c r="G54" s="2"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D55" s="2"/>
       <c r="G55" s="2"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D56" s="2"/>
       <c r="G56" s="2"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D57" s="2"/>
       <c r="G57" s="2"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D58" s="2"/>
       <c r="G58" s="2"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D59" s="2"/>
       <c r="G59" s="2"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D60" s="2"/>
       <c r="G60" s="2"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D61" s="2"/>
       <c r="G61" s="2"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="62" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D62" s="2"/>
       <c r="G62" s="2"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D63" s="2"/>
       <c r="G63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="64" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D64" s="2"/>
       <c r="G64" s="2"/>
       <c r="J64" s="2"/>
     </row>
-    <row r="65" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D65" s="2"/>
       <c r="G65" s="2"/>
       <c r="J65" s="2"/>
     </row>
-    <row r="66" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="66" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D66" s="2"/>
       <c r="G66" s="2"/>
       <c r="J66" s="2"/>
     </row>
-    <row r="67" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="67" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D67" s="2"/>
       <c r="G67" s="2"/>
       <c r="J67" s="2"/>
     </row>
-    <row r="68" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="68" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D68" s="2"/>
       <c r="G68" s="2"/>
       <c r="J68" s="2"/>
     </row>
-    <row r="69" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="69" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D69" s="2"/>
       <c r="G69" s="2"/>
       <c r="J69" s="2"/>
     </row>
-    <row r="70" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="70" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D70" s="2"/>
       <c r="G70" s="2"/>
       <c r="J70" s="2"/>
     </row>
-    <row r="71" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D71" s="2"/>
       <c r="G71" s="2"/>
       <c r="J71" s="2"/>
     </row>
-    <row r="72" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D72" s="2"/>
       <c r="G72" s="2"/>
       <c r="J72" s="2"/>
     </row>
-    <row r="73" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D73" s="2"/>
       <c r="G73" s="2"/>
       <c r="J73" s="2"/>
     </row>
-    <row r="74" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="74" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D74" s="2"/>
       <c r="G74" s="2"/>
       <c r="J74" s="2"/>
     </row>
-    <row r="75" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="75" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D75" s="2"/>
       <c r="G75" s="2"/>
       <c r="J75" s="2"/>
     </row>
-    <row r="76" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="76" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D76" s="2"/>
       <c r="G76" s="2"/>
       <c r="J76" s="2"/>
     </row>
-    <row r="77" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D77" s="2"/>
       <c r="G77" s="2"/>
       <c r="J77" s="2"/>
     </row>
-    <row r="78" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="78" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D78" s="2"/>
       <c r="G78" s="2"/>
       <c r="J78" s="2"/>
     </row>
-    <row r="79" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="79" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D79" s="2"/>
       <c r="G79" s="2"/>
       <c r="J79" s="2"/>
     </row>
-    <row r="80" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="80" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D80" s="2"/>
       <c r="G80" s="2"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="81" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D81" s="2"/>
       <c r="G81" s="2"/>
       <c r="J81" s="2"/>
     </row>
-    <row r="82" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="82" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D82" s="2"/>
       <c r="G82" s="2"/>
       <c r="J82" s="2"/>
     </row>
-    <row r="83" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D83" s="2"/>
       <c r="G83" s="2"/>
       <c r="J83" s="2"/>
     </row>
-    <row r="84" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="84" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D84" s="2"/>
       <c r="G84" s="2"/>
       <c r="J84" s="2"/>
     </row>
-    <row r="85" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="85" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D85" s="2"/>
       <c r="G85" s="2"/>
       <c r="J85" s="2"/>
     </row>
-    <row r="86" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="86" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D86" s="2"/>
       <c r="G86" s="2"/>
       <c r="J86" s="2"/>
     </row>
-    <row r="87" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="87" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D87" s="2"/>
       <c r="G87" s="2"/>
       <c r="J87" s="2"/>
     </row>
-    <row r="88" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="88" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D88" s="2"/>
       <c r="G88" s="2"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="89" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D89" s="2"/>
       <c r="G89" s="2"/>
       <c r="J89" s="2"/>
     </row>
-    <row r="90" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="90" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D90" s="2"/>
       <c r="G90" s="2"/>
       <c r="J90" s="2"/>
     </row>
-    <row r="91" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="91" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D91" s="2"/>
       <c r="G91" s="2"/>
       <c r="J91" s="2"/>
     </row>
-    <row r="92" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="92" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D92" s="2"/>
       <c r="G92" s="2"/>
       <c r="J92" s="2"/>
     </row>
-    <row r="93" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="93" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D93" s="2"/>
       <c r="G93" s="2"/>
       <c r="J93" s="2"/>
     </row>
-    <row r="94" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="94" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D94" s="2"/>
       <c r="G94" s="2"/>
       <c r="J94" s="2"/>
     </row>
-    <row r="95" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="95" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D95" s="2"/>
       <c r="G95" s="2"/>
       <c r="J95" s="2"/>
     </row>
-    <row r="96" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="96" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D96" s="2"/>
       <c r="G96" s="2"/>
       <c r="J96" s="2"/>
     </row>
-    <row r="97" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="97" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D97" s="2"/>
       <c r="G97" s="2"/>
       <c r="J97" s="2"/>
     </row>
-    <row r="98" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="98" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D98" s="2"/>
       <c r="G98" s="2"/>
       <c r="J98" s="2"/>
     </row>
-    <row r="99" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="99" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D99" s="2"/>
       <c r="G99" s="2"/>
       <c r="J99" s="2"/>
     </row>
-    <row r="100" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="100" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D100" s="2"/>
       <c r="G100" s="2"/>
       <c r="J100" s="2"/>
     </row>
-    <row r="101" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="101" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D101" s="2"/>
       <c r="G101" s="2"/>
       <c r="J101" s="2"/>
     </row>
-    <row r="102" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="102" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D102" s="2"/>
       <c r="G102" s="2"/>
       <c r="J102" s="2"/>
     </row>
-    <row r="103" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="103" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D103" s="2"/>
       <c r="G103" s="2"/>
       <c r="J103" s="2"/>
     </row>
-    <row r="104" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="104" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D104" s="2"/>
       <c r="G104" s="2"/>
       <c r="J104" s="2"/>
     </row>
-    <row r="105" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="105" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D105" s="2"/>
       <c r="G105" s="2"/>
       <c r="J105" s="2"/>
     </row>
-    <row r="106" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="106" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D106" s="2"/>
       <c r="G106" s="2"/>
       <c r="J106" s="2"/>
     </row>
-    <row r="107" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="107" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D107" s="2"/>
       <c r="G107" s="2"/>
       <c r="J107" s="2"/>
     </row>
-    <row r="108" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="108" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D108" s="2"/>
       <c r="G108" s="2"/>
       <c r="J108" s="2"/>
     </row>
-    <row r="109" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="109" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D109" s="2"/>
       <c r="G109" s="2"/>
       <c r="J109" s="2"/>
     </row>
-    <row r="110" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="110" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D110" s="2"/>
       <c r="G110" s="2"/>
       <c r="J110" s="2"/>
     </row>
-    <row r="111" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="111" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D111" s="2"/>
       <c r="G111" s="2"/>
       <c r="J111" s="2"/>
     </row>
-    <row r="112" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="112" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D112" s="2"/>
       <c r="G112" s="2"/>
       <c r="J112" s="2"/>
     </row>
-    <row r="113" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="113" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D113" s="2"/>
       <c r="G113" s="2"/>
       <c r="J113" s="2"/>
     </row>
-    <row r="114" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="114" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D114" s="2"/>
       <c r="G114" s="2"/>
       <c r="J114" s="2"/>
     </row>
-    <row r="115" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="115" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D115" s="2"/>
       <c r="G115" s="2"/>
       <c r="J115" s="2"/>
     </row>
-    <row r="116" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="116" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D116" s="2"/>
       <c r="G116" s="2"/>
       <c r="J116" s="2"/>
     </row>
-    <row r="117" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="117" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D117" s="2"/>
       <c r="G117" s="2"/>
       <c r="J117" s="2"/>
     </row>
-    <row r="118" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="118" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D118" s="2"/>
       <c r="G118" s="2"/>
       <c r="J118" s="2"/>
     </row>
-    <row r="119" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="119" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D119" s="2"/>
       <c r="G119" s="2"/>
       <c r="J119" s="2"/>
     </row>
-    <row r="120" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="120" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D120" s="2"/>
       <c r="G120" s="2"/>
       <c r="J120" s="2"/>
     </row>
-    <row r="121" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="121" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D121" s="2"/>
       <c r="G121" s="2"/>
       <c r="J121" s="2"/>
     </row>
-    <row r="122" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="122" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D122" s="2"/>
       <c r="G122" s="2"/>
       <c r="J122" s="2"/>
     </row>
-    <row r="123" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="123" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D123" s="2"/>
       <c r="G123" s="2"/>
       <c r="J123" s="2"/>
     </row>
-    <row r="124" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="124" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D124" s="2"/>
       <c r="G124" s="2"/>
       <c r="J124" s="2"/>
     </row>
-    <row r="125" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="125" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D125" s="2"/>
       <c r="G125" s="2"/>
       <c r="J125" s="2"/>
     </row>
-    <row r="126" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="126" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D126" s="2"/>
       <c r="G126" s="2"/>
       <c r="J126" s="2"/>
     </row>
-    <row r="127" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="127" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D127" s="2"/>
       <c r="G127" s="2"/>
       <c r="J127" s="2"/>
     </row>
-    <row r="128" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="128" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D128" s="2"/>
       <c r="G128" s="2"/>
       <c r="J128" s="2"/>
     </row>
-    <row r="129" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="129" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D129" s="2"/>
       <c r="G129" s="2"/>
       <c r="J129" s="2"/>
     </row>
-    <row r="130" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="130" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D130" s="2"/>
       <c r="G130" s="2"/>
       <c r="J130" s="2"/>
     </row>
-    <row r="131" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="131" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D131" s="2"/>
       <c r="G131" s="2"/>
       <c r="J131" s="2"/>
     </row>
-    <row r="132" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="132" spans="4:10" x14ac:dyDescent="0.35">
       <c r="D132" s="2"/>
       <c r="G132" s="2"/>
       <c r="J132" s="2"/>

</xml_diff>

<commit_message>
Login- und Registration View + Excelsheet
</commit_message>
<xml_diff>
--- a/Excelsheet_Webproject.xlsx
+++ b/Excelsheet_Webproject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forme\OneDrive\Desktop\Schual\SWP\GitHub\NotizenProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00009E13-3992-4562-B94E-ACC59ECE84C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{34C74C50-1293-4BE5-9D85-039682E6FF43}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{00009E13-3992-4562-B94E-ACC59ECE84C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{965D414D-07E6-406D-9914-B861CEE50AC7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FD55CC8F-81FA-4163-8113-51E07961513C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Thema: Website für Notizen und Einträge</t>
   </si>
@@ -66,10 +66,13 @@
     <t>Excelsheet erstellen</t>
   </si>
   <si>
-    <t>Grundlayout deisgned</t>
-  </si>
-  <si>
     <t>User- und Message Klasse</t>
+  </si>
+  <si>
+    <t>UserController + Views erstellt</t>
+  </si>
+  <si>
+    <t>Grundlayout designed</t>
   </si>
 </sst>
 </file>
@@ -512,12 +515,12 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="26.08984375" customWidth="1"/>
+    <col min="8" max="8" width="29.90625" customWidth="1"/>
     <col min="9" max="9" width="10.6328125" style="11"/>
   </cols>
   <sheetData>
@@ -594,7 +597,7 @@
         <v>43846</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>2</v>
@@ -613,7 +616,7 @@
         <v>43846</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>3</v>
@@ -625,7 +628,18 @@
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
-      <c r="G6" s="2"/>
+      <c r="F6" s="8">
+        <v>43846</v>
+      </c>
+      <c r="G6" s="10">
+        <v>43846</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
User Email geaddet und Notizenklasse hinzugefügt
</commit_message>
<xml_diff>
--- a/Excelsheet_Webproject.xlsx
+++ b/Excelsheet_Webproject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forme\OneDrive\Desktop\Schual\SWP\GitHub\NotizenProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{608017D4-BEC7-449F-853E-EB214D6152C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{993959BA-D87D-4834-B753-EA7279C173BE}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{608017D4-BEC7-449F-853E-EB214D6152C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6BF6EBE1-D0AC-44FD-9948-10059B3A3584}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FD55CC8F-81FA-4163-8113-51E07961513C}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <dimension ref="A1:J132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,7 +711,9 @@
       <c r="F9" s="8">
         <v>43859</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="10">
+        <v>43860</v>
+      </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
@@ -728,7 +730,9 @@
       <c r="F10" s="8">
         <v>43859</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="10">
+        <v>43860</v>
+      </c>
       <c r="H10" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Hover-Farbe von Notiz geänder und Excelsheet aufgaben hinzugefügt
</commit_message>
<xml_diff>
--- a/Excelsheet_Webproject.xlsx
+++ b/Excelsheet_Webproject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elias Rist\Documents\GitHub\NotizenProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497B9A86-9FD6-40AF-83DF-64F4ED6F5E6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B39A10-1DC2-4BA2-84E3-1A8C29725E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD55CC8F-81FA-4163-8113-51E07961513C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD55CC8F-81FA-4163-8113-51E07961513C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>Thema: Website für Notizen und Einträge</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Tags hinzufügen, löschen und editieren</t>
+  </si>
+  <si>
+    <t>Multilanguage</t>
+  </si>
+  <si>
+    <t>Tags farben</t>
   </si>
 </sst>
 </file>
@@ -574,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85157E23-AB2B-4896-9F10-4659EA962977}">
   <dimension ref="A1:J133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,6 +1031,9 @@
       <c r="E23" s="8">
         <v>43913</v>
       </c>
+      <c r="F23" s="8">
+        <v>43914</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" t="s">
         <v>30</v>
@@ -1078,12 +1087,30 @@
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
+      <c r="E27" s="8">
+        <v>43914</v>
+      </c>
       <c r="G27" s="2"/>
+      <c r="H27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>2</v>
+      </c>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D28" s="2"/>
+      <c r="E28" s="8">
+        <v>43914</v>
+      </c>
       <c r="G28" s="2"/>
+      <c r="H28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Notizen Farbe wird nun sofort verändert + Code schön strukturiert
Durch Javascript wird die Border-Top-Farbe der Notiz sofort verändert.
Code wurde schön strukturiert
</commit_message>
<xml_diff>
--- a/Excelsheet_Webproject.xlsx
+++ b/Excelsheet_Webproject.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elias Rist\Documents\GitHub\NotizenProjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B39A10-1DC2-4BA2-84E3-1A8C29725E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB944DC-DBA0-4E43-959E-20FC56E360C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD55CC8F-81FA-4163-8113-51E07961513C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD55CC8F-81FA-4163-8113-51E07961513C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -581,7 +581,7 @@
   <dimension ref="A1:J133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,7 +1034,9 @@
       <c r="F23" s="8">
         <v>43914</v>
       </c>
-      <c r="G23" s="2"/>
+      <c r="G23" s="10">
+        <v>43914</v>
+      </c>
       <c r="H23" t="s">
         <v>30</v>
       </c>
@@ -1047,6 +1049,9 @@
       <c r="D24" s="2"/>
       <c r="E24" s="8">
         <v>43913</v>
+      </c>
+      <c r="F24" s="8">
+        <v>43914</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" t="s">

</xml_diff>